<commit_message>
qpp011: update code export
</commit_message>
<xml_diff>
--- a/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/qpp011b.xlsx
+++ b/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/qpp011b.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>住　民　税　納　付　先</t>
     <rPh sb="0" eb="1">
@@ -104,11 +104,15 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
+    <t>【　処理年月 :　　　　　　　　　                                】　</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
     <t>&amp;=header.startResiTaxAutonomy(bean)</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>【　処理年月 :　　　　　　　　　                                】　</t>
+    <t>&amp;=header.date(bean)</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -204,7 +208,9 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -214,23 +220,10 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -239,7 +232,9 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -250,10 +245,25 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -266,7 +276,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -281,38 +291,47 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -637,17 +656,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="17.75" style="5" customWidth="1"/>
     <col min="2" max="2" width="32.625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="31.125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18.25" style="5" customWidth="1"/>
     <col min="4" max="4" width="19.375" style="5" customWidth="1"/>
     <col min="5" max="5" width="20.25" style="5" customWidth="1"/>
     <col min="6" max="6" width="28.25" style="5" customWidth="1"/>
@@ -655,13 +674,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="9" t="s">
+      <c r="B1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -671,27 +690,29 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="A2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="6"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:6" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="3"/>
@@ -705,45 +726,48 @@
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12" t="s">
+      <c r="B6" s="10"/>
+      <c r="C6" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
     </row>
     <row r="8" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="16"/>
     </row>
     <row r="9" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="10" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="B11" s="19"/>
+    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="D8:F8"/>
@@ -756,7 +780,7 @@
   <pageMargins left="0.47244094488188998" right="0.47244094488188998" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
   <pageSetup paperSize="9" scale="90" pageOrder="overThenDown" orientation="landscape" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;L【　日通システム株式会社    】&amp;C&amp;"+,標準"&amp;18住民税チェックリスト（納付先別）&amp;R&amp;"+,標準"&amp;P/&amp;N</oddHeader>
+    <oddHeader>&amp;C&amp;"+,標準"&amp;18住民税チェックリスト（納付先別）&amp;R&amp;"+,標準"&amp;P/&amp;N</oddHeader>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
qpp111: fix template b and fix validate ui
</commit_message>
<xml_diff>
--- a/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/qpp011b.xlsx
+++ b/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/qpp011b.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sonnh\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UK\code v2\nts.uk\file\pr\nts.uk.file.pr.infra\src\main\resources\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -124,11 +124,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -136,7 +136,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -149,7 +149,7 @@
     </font>
     <font>
       <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -163,7 +163,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -286,26 +286,26 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -634,45 +634,45 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C4" sqref="C4:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.25"/>
   <cols>
-    <col min="1" max="1" width="17.75" style="3" customWidth="1"/>
-    <col min="2" max="2" width="32.625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="18.25" style="3" customWidth="1"/>
-    <col min="4" max="4" width="19.375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="20.25" style="3" customWidth="1"/>
-    <col min="6" max="6" width="7.125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" style="3" customWidth="1"/>
     <col min="7" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="26.25" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" s="2" customFormat="1" ht="14.25" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-    </row>
-    <row r="3" spans="1:6" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+    </row>
+    <row r="3" spans="1:6" s="2" customFormat="1" ht="14.25" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -684,29 +684,29 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="12" t="s">
+    <row r="4" spans="1:6" ht="17.25" customHeight="1">
+      <c r="A4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12" t="s">
+      <c r="B4" s="11"/>
+      <c r="C4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-    </row>
-    <row r="5" spans="1:6" ht="1.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-    </row>
-    <row r="6" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+    </row>
+    <row r="5" spans="1:6" ht="1.5" customHeight="1">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+    </row>
+    <row r="6" spans="1:6" ht="20.25" customHeight="1">
       <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
@@ -724,15 +724,15 @@
       </c>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="20.25" customHeight="1">
       <c r="C7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="20.25" customHeight="1"/>
+    <row r="9" spans="1:6">
       <c r="B9" s="5"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6">
       <c r="C11" s="10"/>
     </row>
   </sheetData>

</xml_diff>